<commit_message>
Oct 17. README updated and file reorg
</commit_message>
<xml_diff>
--- a/Nutrient absorption/output.xlsx
+++ b/Nutrient absorption/output.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CE18"/>
+  <dimension ref="A1:CE17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -776,258 +776,258 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1.71115</v>
+        <v>1.6095</v>
       </c>
       <c r="B2">
-        <v>3683953</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>3754919</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>2592344</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>3498643</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>2382097</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>2234823</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>3006634</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>1398395</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>1291221</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>2429163</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>1833449</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>1981569</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>1369367</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>965763</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>5108104</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>1350862</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>1334397</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>2173354</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>2008453</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>1073252</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>626176</v>
+        <v>0</v>
       </c>
       <c r="X2">
-        <v>1392550</v>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <v>1186011</v>
+        <v>0</v>
       </c>
       <c r="Z2">
-        <v>1319952</v>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <v>1147798</v>
+        <v>0</v>
       </c>
       <c r="AB2">
-        <v>1679471</v>
+        <v>0</v>
       </c>
       <c r="AC2">
-        <v>543418</v>
+        <v>0</v>
       </c>
       <c r="AD2">
-        <v>1452859</v>
+        <v>0</v>
       </c>
       <c r="AE2">
-        <v>1725403</v>
+        <v>0</v>
       </c>
       <c r="AF2">
-        <v>1025133</v>
+        <v>0</v>
       </c>
       <c r="AG2">
-        <v>1373497</v>
+        <v>0</v>
       </c>
       <c r="AH2">
-        <v>948478</v>
+        <v>0</v>
       </c>
       <c r="AI2">
-        <v>796309</v>
+        <v>0</v>
       </c>
       <c r="AJ2">
-        <v>1123009</v>
+        <v>0</v>
       </c>
       <c r="AK2">
-        <v>1021142</v>
+        <v>0</v>
       </c>
       <c r="AL2">
-        <v>849380</v>
+        <v>0</v>
       </c>
       <c r="AM2">
-        <v>777335</v>
+        <v>0</v>
       </c>
       <c r="AN2">
-        <v>1443366</v>
+        <v>0</v>
       </c>
       <c r="AO2">
-        <v>791215</v>
+        <v>0</v>
       </c>
       <c r="AP2">
-        <v>992777</v>
+        <v>0</v>
       </c>
       <c r="AQ2">
-        <v>1211055</v>
+        <v>0</v>
       </c>
       <c r="AR2">
-        <v>1067271</v>
+        <v>0</v>
       </c>
       <c r="AS2">
-        <v>808771</v>
+        <v>0</v>
       </c>
       <c r="AT2">
-        <v>903527</v>
+        <v>0</v>
       </c>
       <c r="AU2">
-        <v>962084</v>
+        <v>0</v>
       </c>
       <c r="AV2">
-        <v>1323644</v>
+        <v>0</v>
       </c>
       <c r="AW2">
-        <v>1004365</v>
+        <v>0</v>
       </c>
       <c r="AX2">
-        <v>1303136</v>
+        <v>0</v>
       </c>
       <c r="AY2">
-        <v>942886</v>
+        <v>0</v>
       </c>
       <c r="AZ2">
-        <v>877337</v>
+        <v>0</v>
       </c>
       <c r="BA2">
-        <v>597156</v>
+        <v>0</v>
       </c>
       <c r="BB2">
-        <v>1070703</v>
+        <v>0</v>
       </c>
       <c r="BC2">
-        <v>996864</v>
+        <v>0</v>
       </c>
       <c r="BD2">
-        <v>1468874</v>
+        <v>0</v>
       </c>
       <c r="BE2">
-        <v>1379562</v>
+        <v>0</v>
       </c>
       <c r="BF2">
-        <v>732626</v>
+        <v>0</v>
       </c>
       <c r="BG2">
-        <v>695028</v>
+        <v>0</v>
       </c>
       <c r="BH2">
-        <v>736707</v>
+        <v>0</v>
       </c>
       <c r="BI2">
         <v>693589</v>
       </c>
       <c r="BJ2">
-        <v>717614</v>
+        <v>0</v>
       </c>
       <c r="BK2">
-        <v>661912</v>
+        <v>0</v>
       </c>
       <c r="BL2">
-        <v>570547</v>
+        <v>0</v>
       </c>
       <c r="BM2">
-        <v>846111</v>
+        <v>0</v>
       </c>
       <c r="BN2">
-        <v>691997</v>
+        <v>0</v>
       </c>
       <c r="BO2">
-        <v>761601</v>
+        <v>0</v>
       </c>
       <c r="BP2">
-        <v>607898</v>
+        <v>0</v>
       </c>
       <c r="BQ2">
         <v>0</v>
       </c>
       <c r="BR2">
-        <v>991674</v>
+        <v>0</v>
       </c>
       <c r="BS2">
-        <v>973452</v>
+        <v>0</v>
       </c>
       <c r="BT2">
-        <v>713672</v>
+        <v>0</v>
       </c>
       <c r="BU2">
         <v>397893</v>
       </c>
       <c r="BV2">
-        <v>694711</v>
+        <v>0</v>
       </c>
       <c r="BW2">
-        <v>669762</v>
+        <v>0</v>
       </c>
       <c r="BX2">
-        <v>823497</v>
+        <v>0</v>
       </c>
       <c r="BY2">
-        <v>1139666</v>
+        <v>0</v>
       </c>
       <c r="BZ2">
-        <v>717680</v>
+        <v>0</v>
       </c>
       <c r="CA2">
-        <v>587070</v>
+        <v>0</v>
       </c>
       <c r="CB2">
-        <v>790730</v>
+        <v>0</v>
       </c>
       <c r="CC2">
-        <v>725375</v>
+        <v>0</v>
       </c>
       <c r="CD2">
-        <v>706432</v>
+        <v>0</v>
       </c>
       <c r="CE2">
-        <v>683279</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>1.745</v>
+        <v>1.666364864864865</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1036,273 +1036,273 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>2592344</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>2760701</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>2382097</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>2234823</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1398395</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1291221</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>2429163</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>1833449</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>1981569</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>1369367</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>965763</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>1350862</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>1334397</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>2173354</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>2008453</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>1073252</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>626176</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <v>1392550</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <v>1186011</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <v>1319952</v>
       </c>
       <c r="AA3">
-        <v>0</v>
+        <v>1147798</v>
       </c>
       <c r="AB3">
-        <v>0</v>
+        <v>1679471</v>
       </c>
       <c r="AC3">
-        <v>0</v>
+        <v>543418</v>
       </c>
       <c r="AD3">
-        <v>0</v>
+        <v>1452859</v>
       </c>
       <c r="AE3">
-        <v>0</v>
+        <v>1725403</v>
       </c>
       <c r="AF3">
-        <v>0</v>
+        <v>1025133</v>
       </c>
       <c r="AG3">
-        <v>0</v>
+        <v>1373497</v>
       </c>
       <c r="AH3">
-        <v>0</v>
+        <v>948478</v>
       </c>
       <c r="AI3">
-        <v>0</v>
+        <v>796309</v>
       </c>
       <c r="AJ3">
-        <v>0</v>
+        <v>1123009</v>
       </c>
       <c r="AK3">
-        <v>0</v>
+        <v>1021142</v>
       </c>
       <c r="AL3">
-        <v>0</v>
+        <v>849380</v>
       </c>
       <c r="AM3">
-        <v>0</v>
+        <v>777335</v>
       </c>
       <c r="AN3">
-        <v>0</v>
+        <v>1443366</v>
       </c>
       <c r="AO3">
-        <v>0</v>
+        <v>791215</v>
       </c>
       <c r="AP3">
-        <v>0</v>
+        <v>992777</v>
       </c>
       <c r="AQ3">
-        <v>0</v>
+        <v>1211055</v>
       </c>
       <c r="AR3">
-        <v>0</v>
+        <v>1067271</v>
       </c>
       <c r="AS3">
-        <v>0</v>
+        <v>808771</v>
       </c>
       <c r="AT3">
-        <v>0</v>
+        <v>903527</v>
       </c>
       <c r="AU3">
-        <v>0</v>
+        <v>962084</v>
       </c>
       <c r="AV3">
-        <v>0</v>
+        <v>1323644</v>
       </c>
       <c r="AW3">
-        <v>0</v>
+        <v>1004365</v>
       </c>
       <c r="AX3">
-        <v>0</v>
+        <v>1303136</v>
       </c>
       <c r="AY3">
-        <v>0</v>
+        <v>942886</v>
       </c>
       <c r="AZ3">
-        <v>0</v>
+        <v>877337</v>
       </c>
       <c r="BA3">
-        <v>0</v>
+        <v>597156</v>
       </c>
       <c r="BB3">
-        <v>0</v>
+        <v>1070703</v>
       </c>
       <c r="BC3">
-        <v>0</v>
+        <v>996864</v>
       </c>
       <c r="BD3">
-        <v>0</v>
+        <v>1468874</v>
       </c>
       <c r="BE3">
-        <v>0</v>
+        <v>1379562</v>
       </c>
       <c r="BF3">
-        <v>0</v>
+        <v>732626</v>
       </c>
       <c r="BG3">
-        <v>0</v>
+        <v>695028</v>
       </c>
       <c r="BH3">
-        <v>0</v>
+        <v>736707</v>
       </c>
       <c r="BI3">
         <v>0</v>
       </c>
       <c r="BJ3">
-        <v>0</v>
+        <v>717614</v>
       </c>
       <c r="BK3">
-        <v>0</v>
+        <v>661912</v>
       </c>
       <c r="BL3">
-        <v>0</v>
+        <v>570547</v>
       </c>
       <c r="BM3">
-        <v>0</v>
+        <v>846111</v>
       </c>
       <c r="BN3">
-        <v>0</v>
+        <v>691997</v>
       </c>
       <c r="BO3">
-        <v>0</v>
+        <v>761601</v>
       </c>
       <c r="BP3">
-        <v>0</v>
+        <v>607898</v>
       </c>
       <c r="BQ3">
         <v>1156207</v>
       </c>
       <c r="BR3">
-        <v>0</v>
+        <v>991674</v>
       </c>
       <c r="BS3">
-        <v>0</v>
+        <v>973452</v>
       </c>
       <c r="BT3">
-        <v>0</v>
+        <v>713672</v>
       </c>
       <c r="BU3">
         <v>0</v>
       </c>
       <c r="BV3">
-        <v>0</v>
+        <v>694711</v>
       </c>
       <c r="BW3">
-        <v>0</v>
+        <v>669762</v>
       </c>
       <c r="BX3">
-        <v>0</v>
+        <v>823497</v>
       </c>
       <c r="BY3">
-        <v>0</v>
+        <v>1139666</v>
       </c>
       <c r="BZ3">
-        <v>0</v>
+        <v>717680</v>
       </c>
       <c r="CA3">
-        <v>0</v>
+        <v>587070</v>
       </c>
       <c r="CB3">
-        <v>0</v>
+        <v>790730</v>
       </c>
       <c r="CC3">
-        <v>0</v>
+        <v>725375</v>
       </c>
       <c r="CD3">
-        <v>0</v>
+        <v>706432</v>
       </c>
       <c r="CE3">
-        <v>0</v>
+        <v>683279</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>1.894714285714286</v>
+        <v>1.725</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>3683953</v>
       </c>
       <c r="C4">
-        <v>162211</v>
+        <v>3754919</v>
       </c>
       <c r="D4">
-        <v>117175</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>54482</v>
+        <v>3498643</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>2760701</v>
       </c>
       <c r="G4">
-        <v>34166</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>33682</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>3006634</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1311,7 +1311,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>46868</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -1335,7 +1335,7 @@
         <v>0</v>
       </c>
       <c r="T4">
-        <v>10361</v>
+        <v>0</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -1529,10 +1529,10 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>1.935</v>
+        <v>1.767</v>
       </c>
       <c r="B5">
-        <v>120129</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1544,7 +1544,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>38421</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1556,31 +1556,31 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>49417</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>29327</v>
+        <v>0</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>24833</v>
+        <v>0</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
       <c r="O5">
-        <v>37476</v>
+        <v>0</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>121681</v>
+        <v>5108104</v>
       </c>
       <c r="R5">
-        <v>66993</v>
+        <v>0</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -1598,13 +1598,13 @@
         <v>0</v>
       </c>
       <c r="X5">
-        <v>42317</v>
+        <v>0</v>
       </c>
       <c r="Y5">
         <v>0</v>
       </c>
       <c r="Z5">
-        <v>47936</v>
+        <v>0</v>
       </c>
       <c r="AA5">
         <v>0</v>
@@ -1619,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="AE5">
-        <v>17306</v>
+        <v>0</v>
       </c>
       <c r="AF5">
         <v>0</v>
@@ -1780,49 +1780,49 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>1.9875</v>
+        <v>1.8915625</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>162211</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>117175</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>54482</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>38421</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>34166</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>33682</v>
       </c>
       <c r="I6">
-        <v>140013</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>49417</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>29327</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>46868</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>24833</v>
       </c>
       <c r="N6">
         <v>0</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>37476</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1831,13 +1831,13 @@
         <v>0</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>66993</v>
       </c>
       <c r="S6">
         <v>0</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>10361</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -1849,13 +1849,13 @@
         <v>0</v>
       </c>
       <c r="X6">
-        <v>0</v>
+        <v>42317</v>
       </c>
       <c r="Y6">
         <v>0</v>
       </c>
       <c r="Z6">
-        <v>0</v>
+        <v>47936</v>
       </c>
       <c r="AA6">
         <v>0</v>
@@ -1870,7 +1870,7 @@
         <v>0</v>
       </c>
       <c r="AE6">
-        <v>14365</v>
+        <v>17306</v>
       </c>
       <c r="AF6">
         <v>0</v>
@@ -2031,16 +2031,16 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>2.061666666666667</v>
+        <v>1.9695</v>
       </c>
       <c r="B7">
-        <v>90368</v>
+        <v>120129</v>
       </c>
       <c r="C7">
-        <v>172277</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>74730</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2055,7 +2055,7 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>140013</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -2079,7 +2079,7 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>121681</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -2121,7 +2121,7 @@
         <v>0</v>
       </c>
       <c r="AE7">
-        <v>0</v>
+        <v>14365</v>
       </c>
       <c r="AF7">
         <v>0</v>
@@ -2282,16 +2282,16 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>2.097</v>
+        <v>2.053</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>90368</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>74730</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -2330,7 +2330,7 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>137281</v>
+        <v>0</v>
       </c>
       <c r="R8">
         <v>0</v>
@@ -2533,31 +2533,31 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>3.6418</v>
+        <v>2.089</v>
       </c>
       <c r="B9">
-        <v>372867</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>570143</v>
+        <v>172277</v>
       </c>
       <c r="D9">
-        <v>1272107</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>172158</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>168976</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>409703</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>4799237</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -2566,7 +2566,7 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>91734</v>
+        <v>0</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -2581,7 +2581,7 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>523969</v>
+        <v>0</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -2590,7 +2590,7 @@
         <v>0</v>
       </c>
       <c r="T9">
-        <v>222646</v>
+        <v>0</v>
       </c>
       <c r="U9">
         <v>0</v>
@@ -2784,7 +2784,7 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>3.692377049180328</v>
+        <v>2.127</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -2799,7 +2799,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>697485</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -2811,31 +2811,31 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>134006</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>290503</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>109133</v>
+        <v>0</v>
       </c>
       <c r="N10">
         <v>0</v>
       </c>
       <c r="O10">
-        <v>134447</v>
+        <v>0</v>
       </c>
       <c r="P10">
-        <v>831730</v>
+        <v>0</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>137281</v>
       </c>
       <c r="R10">
-        <v>160351</v>
+        <v>0</v>
       </c>
       <c r="S10">
         <v>0</v>
@@ -2844,25 +2844,25 @@
         <v>0</v>
       </c>
       <c r="U10">
-        <v>131686</v>
+        <v>0</v>
       </c>
       <c r="V10">
-        <v>390107</v>
+        <v>0</v>
       </c>
       <c r="W10">
         <v>0</v>
       </c>
       <c r="X10">
-        <v>226554</v>
+        <v>0</v>
       </c>
       <c r="Y10">
         <v>0</v>
       </c>
       <c r="Z10">
-        <v>113636</v>
+        <v>0</v>
       </c>
       <c r="AA10">
-        <v>90939</v>
+        <v>0</v>
       </c>
       <c r="AB10">
         <v>0</v>
@@ -2871,94 +2871,94 @@
         <v>0</v>
       </c>
       <c r="AD10">
-        <v>157253</v>
+        <v>0</v>
       </c>
       <c r="AE10">
-        <v>532666</v>
+        <v>0</v>
       </c>
       <c r="AF10">
-        <v>45788</v>
+        <v>0</v>
       </c>
       <c r="AG10">
-        <v>185459</v>
+        <v>0</v>
       </c>
       <c r="AH10">
-        <v>79237</v>
+        <v>0</v>
       </c>
       <c r="AI10">
-        <v>62577</v>
+        <v>0</v>
       </c>
       <c r="AJ10">
-        <v>436670</v>
+        <v>0</v>
       </c>
       <c r="AK10">
-        <v>360715</v>
+        <v>0</v>
       </c>
       <c r="AL10">
-        <v>47678</v>
+        <v>0</v>
       </c>
       <c r="AM10">
         <v>0</v>
       </c>
       <c r="AN10">
-        <v>110861</v>
+        <v>0</v>
       </c>
       <c r="AO10">
         <v>0</v>
       </c>
       <c r="AP10">
-        <v>74331</v>
+        <v>0</v>
       </c>
       <c r="AQ10">
-        <v>239577</v>
+        <v>0</v>
       </c>
       <c r="AR10">
-        <v>74134</v>
+        <v>0</v>
       </c>
       <c r="AS10">
-        <v>219056</v>
+        <v>0</v>
       </c>
       <c r="AT10">
-        <v>140659</v>
+        <v>0</v>
       </c>
       <c r="AU10">
-        <v>108411</v>
+        <v>0</v>
       </c>
       <c r="AV10">
-        <v>191003</v>
+        <v>0</v>
       </c>
       <c r="AW10">
-        <v>508992</v>
+        <v>0</v>
       </c>
       <c r="AX10">
-        <v>151376</v>
+        <v>0</v>
       </c>
       <c r="AY10">
-        <v>167188</v>
+        <v>0</v>
       </c>
       <c r="AZ10">
-        <v>123444</v>
+        <v>0</v>
       </c>
       <c r="BA10">
-        <v>173459</v>
+        <v>0</v>
       </c>
       <c r="BB10">
-        <v>501929</v>
+        <v>0</v>
       </c>
       <c r="BC10">
-        <v>160957</v>
+        <v>0</v>
       </c>
       <c r="BD10">
-        <v>74141</v>
+        <v>0</v>
       </c>
       <c r="BE10">
-        <v>126055</v>
+        <v>0</v>
       </c>
       <c r="BF10">
-        <v>147644</v>
+        <v>0</v>
       </c>
       <c r="BG10">
-        <v>70542</v>
+        <v>0</v>
       </c>
       <c r="BH10">
         <v>0</v>
@@ -2967,153 +2967,153 @@
         <v>0</v>
       </c>
       <c r="BJ10">
-        <v>62112</v>
+        <v>0</v>
       </c>
       <c r="BK10">
-        <v>144953</v>
+        <v>0</v>
       </c>
       <c r="BL10">
-        <v>205125</v>
+        <v>0</v>
       </c>
       <c r="BM10">
-        <v>59466</v>
+        <v>0</v>
       </c>
       <c r="BN10">
         <v>0</v>
       </c>
       <c r="BO10">
-        <v>67852</v>
+        <v>0</v>
       </c>
       <c r="BP10">
-        <v>53742</v>
+        <v>0</v>
       </c>
       <c r="BQ10">
-        <v>224633</v>
+        <v>0</v>
       </c>
       <c r="BR10">
-        <v>88302</v>
+        <v>0</v>
       </c>
       <c r="BS10">
-        <v>80155</v>
+        <v>0</v>
       </c>
       <c r="BT10">
-        <v>54739</v>
+        <v>0</v>
       </c>
       <c r="BU10">
-        <v>123059</v>
+        <v>0</v>
       </c>
       <c r="BV10">
-        <v>180328</v>
+        <v>0</v>
       </c>
       <c r="BW10">
-        <v>84950</v>
+        <v>0</v>
       </c>
       <c r="BX10">
-        <v>51631</v>
+        <v>0</v>
       </c>
       <c r="BY10">
-        <v>89725</v>
+        <v>0</v>
       </c>
       <c r="BZ10">
-        <v>116768</v>
+        <v>0</v>
       </c>
       <c r="CA10">
-        <v>74738</v>
+        <v>0</v>
       </c>
       <c r="CB10">
-        <v>87013</v>
+        <v>0</v>
       </c>
       <c r="CC10">
-        <v>71495</v>
+        <v>0</v>
       </c>
       <c r="CD10">
-        <v>87958</v>
+        <v>0</v>
       </c>
       <c r="CE10">
-        <v>345189</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>3.913888888888889</v>
+        <v>3.644408450704225</v>
       </c>
       <c r="B11">
-        <v>511218</v>
+        <v>372867</v>
       </c>
       <c r="C11">
-        <v>650159</v>
+        <v>570143</v>
       </c>
       <c r="D11">
-        <v>1327188</v>
+        <v>1272107</v>
       </c>
       <c r="E11">
-        <v>227408</v>
+        <v>172158</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>697485</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>168976</v>
       </c>
       <c r="H11">
-        <v>427960</v>
+        <v>409703</v>
       </c>
       <c r="I11">
-        <v>4139463</v>
+        <v>4799237</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>134006</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>290503</v>
       </c>
       <c r="L11">
-        <v>154197</v>
+        <v>91734</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>109133</v>
       </c>
       <c r="N11">
         <v>0</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>134447</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>831730</v>
       </c>
       <c r="Q11">
-        <v>800293</v>
+        <v>523969</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>160351</v>
       </c>
       <c r="S11">
         <v>0</v>
       </c>
       <c r="T11">
-        <v>431977</v>
+        <v>222646</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>131686</v>
       </c>
       <c r="V11">
-        <v>0</v>
+        <v>390107</v>
       </c>
       <c r="W11">
         <v>0</v>
       </c>
       <c r="X11">
-        <v>0</v>
+        <v>226554</v>
       </c>
       <c r="Y11">
         <v>0</v>
       </c>
       <c r="Z11">
-        <v>0</v>
+        <v>113636</v>
       </c>
       <c r="AA11">
-        <v>0</v>
+        <v>90939</v>
       </c>
       <c r="AB11">
         <v>0</v>
@@ -3122,94 +3122,94 @@
         <v>0</v>
       </c>
       <c r="AD11">
-        <v>0</v>
+        <v>157253</v>
       </c>
       <c r="AE11">
-        <v>0</v>
+        <v>532666</v>
       </c>
       <c r="AF11">
-        <v>0</v>
+        <v>45788</v>
       </c>
       <c r="AG11">
-        <v>0</v>
+        <v>185459</v>
       </c>
       <c r="AH11">
-        <v>0</v>
+        <v>79237</v>
       </c>
       <c r="AI11">
-        <v>0</v>
+        <v>62577</v>
       </c>
       <c r="AJ11">
-        <v>0</v>
+        <v>436670</v>
       </c>
       <c r="AK11">
-        <v>0</v>
+        <v>360715</v>
       </c>
       <c r="AL11">
-        <v>0</v>
+        <v>47678</v>
       </c>
       <c r="AM11">
         <v>0</v>
       </c>
       <c r="AN11">
-        <v>0</v>
+        <v>110861</v>
       </c>
       <c r="AO11">
         <v>0</v>
       </c>
       <c r="AP11">
-        <v>0</v>
+        <v>74331</v>
       </c>
       <c r="AQ11">
-        <v>0</v>
+        <v>239577</v>
       </c>
       <c r="AR11">
-        <v>0</v>
+        <v>74134</v>
       </c>
       <c r="AS11">
-        <v>0</v>
+        <v>219056</v>
       </c>
       <c r="AT11">
-        <v>0</v>
+        <v>140659</v>
       </c>
       <c r="AU11">
-        <v>0</v>
+        <v>108411</v>
       </c>
       <c r="AV11">
-        <v>0</v>
+        <v>191003</v>
       </c>
       <c r="AW11">
-        <v>0</v>
+        <v>508992</v>
       </c>
       <c r="AX11">
-        <v>0</v>
+        <v>151376</v>
       </c>
       <c r="AY11">
-        <v>0</v>
+        <v>167188</v>
       </c>
       <c r="AZ11">
-        <v>0</v>
+        <v>123444</v>
       </c>
       <c r="BA11">
-        <v>0</v>
+        <v>173459</v>
       </c>
       <c r="BB11">
-        <v>0</v>
+        <v>501929</v>
       </c>
       <c r="BC11">
-        <v>0</v>
+        <v>160957</v>
       </c>
       <c r="BD11">
-        <v>0</v>
+        <v>74141</v>
       </c>
       <c r="BE11">
-        <v>0</v>
+        <v>126055</v>
       </c>
       <c r="BF11">
-        <v>0</v>
+        <v>147644</v>
       </c>
       <c r="BG11">
-        <v>0</v>
+        <v>70542</v>
       </c>
       <c r="BH11">
         <v>0</v>
@@ -3218,87 +3218,87 @@
         <v>0</v>
       </c>
       <c r="BJ11">
-        <v>0</v>
+        <v>62112</v>
       </c>
       <c r="BK11">
-        <v>0</v>
+        <v>144953</v>
       </c>
       <c r="BL11">
-        <v>0</v>
+        <v>205125</v>
       </c>
       <c r="BM11">
-        <v>0</v>
+        <v>59466</v>
       </c>
       <c r="BN11">
         <v>0</v>
       </c>
       <c r="BO11">
-        <v>0</v>
+        <v>67852</v>
       </c>
       <c r="BP11">
-        <v>0</v>
+        <v>53742</v>
       </c>
       <c r="BQ11">
-        <v>0</v>
+        <v>224633</v>
       </c>
       <c r="BR11">
-        <v>0</v>
+        <v>88302</v>
       </c>
       <c r="BS11">
-        <v>0</v>
+        <v>80155</v>
       </c>
       <c r="BT11">
-        <v>0</v>
+        <v>54739</v>
       </c>
       <c r="BU11">
-        <v>0</v>
+        <v>123059</v>
       </c>
       <c r="BV11">
-        <v>0</v>
+        <v>180328</v>
       </c>
       <c r="BW11">
-        <v>0</v>
+        <v>84950</v>
       </c>
       <c r="BX11">
-        <v>0</v>
+        <v>51631</v>
       </c>
       <c r="BY11">
-        <v>0</v>
+        <v>89725</v>
       </c>
       <c r="BZ11">
-        <v>0</v>
+        <v>116768</v>
       </c>
       <c r="CA11">
-        <v>0</v>
+        <v>74738</v>
       </c>
       <c r="CB11">
-        <v>0</v>
+        <v>87013</v>
       </c>
       <c r="CC11">
-        <v>0</v>
+        <v>71495</v>
       </c>
       <c r="CD11">
-        <v>0</v>
+        <v>87958</v>
       </c>
       <c r="CE11">
-        <v>0</v>
+        <v>345189</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>3.967591549295774</v>
+        <v>3.91955</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>511218</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>650159</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1327188</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>227408</v>
       </c>
       <c r="F12">
         <v>670293</v>
@@ -3307,10 +3307,10 @@
         <v>183648</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>427960</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>4139463</v>
       </c>
       <c r="J12">
         <v>171490</v>
@@ -3319,7 +3319,7 @@
         <v>342639</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>154197</v>
       </c>
       <c r="M12">
         <v>177924</v>
@@ -3334,7 +3334,7 @@
         <v>838922</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>800293</v>
       </c>
       <c r="R12">
         <v>238798</v>
@@ -3343,7 +3343,7 @@
         <v>76126</v>
       </c>
       <c r="T12">
-        <v>0</v>
+        <v>431977</v>
       </c>
       <c r="U12">
         <v>213735</v>
@@ -3537,7 +3537,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>4.122599999999999</v>
+        <v>4.1162</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -3585,7 +3585,7 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>96994</v>
+        <v>0</v>
       </c>
       <c r="R13">
         <v>0</v>
@@ -3627,7 +3627,7 @@
         <v>0</v>
       </c>
       <c r="AE13">
-        <v>0</v>
+        <v>99892</v>
       </c>
       <c r="AF13">
         <v>0</v>
@@ -3788,7 +3788,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>4.187666666666667</v>
+        <v>4.151666666666666</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -3836,7 +3836,7 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>96994</v>
       </c>
       <c r="R14">
         <v>99301</v>
@@ -3878,7 +3878,7 @@
         <v>0</v>
       </c>
       <c r="AE14">
-        <v>99892</v>
+        <v>0</v>
       </c>
       <c r="AF14">
         <v>0</v>
@@ -4039,7 +4039,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>4.368333333333333</v>
+        <v>4.321666666666667</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4290,7 +4290,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>4.42975</v>
+        <v>4.436909090909091</v>
       </c>
       <c r="B16">
         <v>799427</v>
@@ -4317,7 +4317,7 @@
         <v>847706</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>143825</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -4326,31 +4326,31 @@
         <v>774397</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>239307</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>860679</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>132232</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>230714</v>
       </c>
       <c r="Q16">
         <v>826893</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>573846</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <v>256190</v>
       </c>
       <c r="T16">
         <v>447222</v>
       </c>
       <c r="U16">
-        <v>0</v>
+        <v>692801</v>
       </c>
       <c r="V16">
         <v>202396</v>
@@ -4362,16 +4362,16 @@
         <v>0</v>
       </c>
       <c r="Y16">
-        <v>0</v>
+        <v>201564</v>
       </c>
       <c r="Z16">
         <v>0</v>
       </c>
       <c r="AA16">
-        <v>0</v>
+        <v>188490</v>
       </c>
       <c r="AB16">
-        <v>0</v>
+        <v>333790</v>
       </c>
       <c r="AC16">
         <v>0</v>
@@ -4398,28 +4398,28 @@
         <v>0</v>
       </c>
       <c r="AK16">
-        <v>0</v>
+        <v>247505</v>
       </c>
       <c r="AL16">
-        <v>0</v>
+        <v>120000</v>
       </c>
       <c r="AM16">
-        <v>0</v>
+        <v>92094</v>
       </c>
       <c r="AN16">
-        <v>0</v>
+        <v>327443</v>
       </c>
       <c r="AO16">
-        <v>0</v>
+        <v>128343</v>
       </c>
       <c r="AP16">
-        <v>0</v>
+        <v>173864</v>
       </c>
       <c r="AQ16">
-        <v>0</v>
+        <v>176207</v>
       </c>
       <c r="AR16">
-        <v>0</v>
+        <v>122377</v>
       </c>
       <c r="AS16">
         <v>0</v>
@@ -4437,7 +4437,7 @@
         <v>0</v>
       </c>
       <c r="AX16">
-        <v>0</v>
+        <v>139753</v>
       </c>
       <c r="AY16">
         <v>0</v>
@@ -4452,55 +4452,55 @@
         <v>0</v>
       </c>
       <c r="BC16">
-        <v>0</v>
+        <v>169408</v>
       </c>
       <c r="BD16">
-        <v>0</v>
+        <v>319117</v>
       </c>
       <c r="BE16">
-        <v>0</v>
+        <v>207318</v>
       </c>
       <c r="BF16">
-        <v>0</v>
+        <v>120535</v>
       </c>
       <c r="BG16">
-        <v>0</v>
+        <v>209539</v>
       </c>
       <c r="BH16">
         <v>0</v>
       </c>
       <c r="BI16">
-        <v>0</v>
+        <v>124865</v>
       </c>
       <c r="BJ16">
         <v>0</v>
       </c>
       <c r="BK16">
-        <v>0</v>
+        <v>120590</v>
       </c>
       <c r="BL16">
         <v>0</v>
       </c>
       <c r="BM16">
-        <v>0</v>
+        <v>204136</v>
       </c>
       <c r="BN16">
-        <v>0</v>
+        <v>112784</v>
       </c>
       <c r="BO16">
         <v>0</v>
       </c>
       <c r="BP16">
-        <v>0</v>
+        <v>104300</v>
       </c>
       <c r="BQ16">
         <v>0</v>
       </c>
       <c r="BR16">
-        <v>0</v>
+        <v>122842</v>
       </c>
       <c r="BS16">
-        <v>0</v>
+        <v>106609</v>
       </c>
       <c r="BT16">
         <v>0</v>
@@ -4541,13 +4541,13 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>4.49084375</v>
+        <v>6.239199999999999</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>49565</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>84797</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -4562,13 +4562,13 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>47778</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17">
-        <v>143825</v>
+        <v>0</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -4577,31 +4577,31 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <v>239307</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>860679</v>
+        <v>0</v>
       </c>
       <c r="O17">
-        <v>132232</v>
+        <v>0</v>
       </c>
       <c r="P17">
-        <v>230714</v>
+        <v>0</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>48407</v>
       </c>
       <c r="R17">
-        <v>573846</v>
+        <v>0</v>
       </c>
       <c r="S17">
-        <v>256190</v>
+        <v>0</v>
       </c>
       <c r="T17">
-        <v>0</v>
+        <v>60469</v>
       </c>
       <c r="U17">
-        <v>692801</v>
+        <v>0</v>
       </c>
       <c r="V17">
         <v>0</v>
@@ -4613,16 +4613,16 @@
         <v>0</v>
       </c>
       <c r="Y17">
-        <v>201564</v>
+        <v>0</v>
       </c>
       <c r="Z17">
         <v>0</v>
       </c>
       <c r="AA17">
-        <v>188490</v>
+        <v>0</v>
       </c>
       <c r="AB17">
-        <v>333790</v>
+        <v>0</v>
       </c>
       <c r="AC17">
         <v>0</v>
@@ -4649,28 +4649,28 @@
         <v>0</v>
       </c>
       <c r="AK17">
-        <v>247505</v>
+        <v>0</v>
       </c>
       <c r="AL17">
-        <v>120000</v>
+        <v>0</v>
       </c>
       <c r="AM17">
-        <v>92094</v>
+        <v>0</v>
       </c>
       <c r="AN17">
-        <v>327443</v>
+        <v>0</v>
       </c>
       <c r="AO17">
-        <v>128343</v>
+        <v>0</v>
       </c>
       <c r="AP17">
-        <v>173864</v>
+        <v>0</v>
       </c>
       <c r="AQ17">
-        <v>176207</v>
+        <v>0</v>
       </c>
       <c r="AR17">
-        <v>122377</v>
+        <v>0</v>
       </c>
       <c r="AS17">
         <v>0</v>
@@ -4688,7 +4688,7 @@
         <v>0</v>
       </c>
       <c r="AX17">
-        <v>139753</v>
+        <v>0</v>
       </c>
       <c r="AY17">
         <v>0</v>
@@ -4703,55 +4703,55 @@
         <v>0</v>
       </c>
       <c r="BC17">
-        <v>169408</v>
+        <v>0</v>
       </c>
       <c r="BD17">
-        <v>319117</v>
+        <v>0</v>
       </c>
       <c r="BE17">
-        <v>207318</v>
+        <v>0</v>
       </c>
       <c r="BF17">
-        <v>120535</v>
+        <v>0</v>
       </c>
       <c r="BG17">
-        <v>209539</v>
+        <v>0</v>
       </c>
       <c r="BH17">
         <v>0</v>
       </c>
       <c r="BI17">
-        <v>124865</v>
+        <v>0</v>
       </c>
       <c r="BJ17">
         <v>0</v>
       </c>
       <c r="BK17">
-        <v>120590</v>
+        <v>0</v>
       </c>
       <c r="BL17">
         <v>0</v>
       </c>
       <c r="BM17">
-        <v>204136</v>
+        <v>0</v>
       </c>
       <c r="BN17">
-        <v>112784</v>
+        <v>0</v>
       </c>
       <c r="BO17">
         <v>0</v>
       </c>
       <c r="BP17">
-        <v>104300</v>
+        <v>0</v>
       </c>
       <c r="BQ17">
         <v>0</v>
       </c>
       <c r="BR17">
-        <v>122842</v>
+        <v>0</v>
       </c>
       <c r="BS17">
-        <v>106609</v>
+        <v>0</v>
       </c>
       <c r="BT17">
         <v>0</v>
@@ -4787,257 +4787,6 @@
         <v>0</v>
       </c>
       <c r="CE17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18">
-        <v>6.2272</v>
-      </c>
-      <c r="B18">
-        <v>49565</v>
-      </c>
-      <c r="C18">
-        <v>84797</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>47778</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>48407</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18">
-        <v>60469</v>
-      </c>
-      <c r="U18">
-        <v>0</v>
-      </c>
-      <c r="V18">
-        <v>0</v>
-      </c>
-      <c r="W18">
-        <v>0</v>
-      </c>
-      <c r="X18">
-        <v>0</v>
-      </c>
-      <c r="Y18">
-        <v>0</v>
-      </c>
-      <c r="Z18">
-        <v>0</v>
-      </c>
-      <c r="AA18">
-        <v>0</v>
-      </c>
-      <c r="AB18">
-        <v>0</v>
-      </c>
-      <c r="AC18">
-        <v>0</v>
-      </c>
-      <c r="AD18">
-        <v>0</v>
-      </c>
-      <c r="AE18">
-        <v>0</v>
-      </c>
-      <c r="AF18">
-        <v>0</v>
-      </c>
-      <c r="AG18">
-        <v>0</v>
-      </c>
-      <c r="AH18">
-        <v>0</v>
-      </c>
-      <c r="AI18">
-        <v>0</v>
-      </c>
-      <c r="AJ18">
-        <v>0</v>
-      </c>
-      <c r="AK18">
-        <v>0</v>
-      </c>
-      <c r="AL18">
-        <v>0</v>
-      </c>
-      <c r="AM18">
-        <v>0</v>
-      </c>
-      <c r="AN18">
-        <v>0</v>
-      </c>
-      <c r="AO18">
-        <v>0</v>
-      </c>
-      <c r="AP18">
-        <v>0</v>
-      </c>
-      <c r="AQ18">
-        <v>0</v>
-      </c>
-      <c r="AR18">
-        <v>0</v>
-      </c>
-      <c r="AS18">
-        <v>0</v>
-      </c>
-      <c r="AT18">
-        <v>0</v>
-      </c>
-      <c r="AU18">
-        <v>0</v>
-      </c>
-      <c r="AV18">
-        <v>0</v>
-      </c>
-      <c r="AW18">
-        <v>0</v>
-      </c>
-      <c r="AX18">
-        <v>0</v>
-      </c>
-      <c r="AY18">
-        <v>0</v>
-      </c>
-      <c r="AZ18">
-        <v>0</v>
-      </c>
-      <c r="BA18">
-        <v>0</v>
-      </c>
-      <c r="BB18">
-        <v>0</v>
-      </c>
-      <c r="BC18">
-        <v>0</v>
-      </c>
-      <c r="BD18">
-        <v>0</v>
-      </c>
-      <c r="BE18">
-        <v>0</v>
-      </c>
-      <c r="BF18">
-        <v>0</v>
-      </c>
-      <c r="BG18">
-        <v>0</v>
-      </c>
-      <c r="BH18">
-        <v>0</v>
-      </c>
-      <c r="BI18">
-        <v>0</v>
-      </c>
-      <c r="BJ18">
-        <v>0</v>
-      </c>
-      <c r="BK18">
-        <v>0</v>
-      </c>
-      <c r="BL18">
-        <v>0</v>
-      </c>
-      <c r="BM18">
-        <v>0</v>
-      </c>
-      <c r="BN18">
-        <v>0</v>
-      </c>
-      <c r="BO18">
-        <v>0</v>
-      </c>
-      <c r="BP18">
-        <v>0</v>
-      </c>
-      <c r="BQ18">
-        <v>0</v>
-      </c>
-      <c r="BR18">
-        <v>0</v>
-      </c>
-      <c r="BS18">
-        <v>0</v>
-      </c>
-      <c r="BT18">
-        <v>0</v>
-      </c>
-      <c r="BU18">
-        <v>0</v>
-      </c>
-      <c r="BV18">
-        <v>0</v>
-      </c>
-      <c r="BW18">
-        <v>0</v>
-      </c>
-      <c r="BX18">
-        <v>0</v>
-      </c>
-      <c r="BY18">
-        <v>0</v>
-      </c>
-      <c r="BZ18">
-        <v>0</v>
-      </c>
-      <c r="CA18">
-        <v>0</v>
-      </c>
-      <c r="CB18">
-        <v>0</v>
-      </c>
-      <c r="CC18">
-        <v>0</v>
-      </c>
-      <c r="CD18">
-        <v>0</v>
-      </c>
-      <c r="CE18">
         <v>0</v>
       </c>
     </row>

</xml_diff>